<commit_message>
Fixed the date issue with the BA test data
</commit_message>
<xml_diff>
--- a/doc/student_data/Student_data_workings.xlsx
+++ b/doc/student_data/Student_data_workings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d0f90ebdaed1ff47/15. Studies/UNE/1. MOODLE/Y4T1 - COSC320 Information Technology Project/Cosc320_Group_Project/doc/student_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="8_{525C0C1F-2C98-49F2-9D26-E643EE38A02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14E548B9-472A-4C39-9C58-0F2E8D1CA6E3}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="8_{525C0C1F-2C98-49F2-9D26-E643EE38A02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40F35DDD-D7F9-4BA7-9CD9-A877A8C41C56}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E3029FD-3594-4E3A-BFC9-B8249B0E57B2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9E3029FD-3594-4E3A-BFC9-B8249B0E57B2}"/>
   </bookViews>
   <sheets>
     <sheet name="BA" sheetId="1" r:id="rId1"/>
@@ -11419,8 +11419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66D04577-8695-417A-9A4A-0F8BBA4592AD}">
   <dimension ref="A1:U262"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11528,7 +11528,7 @@
       <c r="H2" t="s">
         <v>25</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="2">
         <v>43528</v>
       </c>
       <c r="J2" t="s">
@@ -11590,7 +11590,7 @@
       <c r="H3" t="s">
         <v>25</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="2">
         <v>44375</v>
       </c>
       <c r="J3" t="s">
@@ -11646,7 +11646,7 @@
       <c r="H4" t="s">
         <v>25</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="2">
         <v>44375</v>
       </c>
       <c r="J4" t="s">
@@ -11705,7 +11705,7 @@
       <c r="H5" t="s">
         <v>25</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="2">
         <v>44226</v>
       </c>
       <c r="J5" t="s">
@@ -11767,7 +11767,7 @@
       <c r="H6" t="s">
         <v>25</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="2">
         <v>44494</v>
       </c>
       <c r="J6" t="s">
@@ -11826,7 +11826,7 @@
       <c r="H7" t="s">
         <v>25</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="2">
         <v>44375</v>
       </c>
       <c r="J7" t="s">
@@ -11885,7 +11885,7 @@
       <c r="H8" t="s">
         <v>25</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="2">
         <v>44259</v>
       </c>
       <c r="J8" t="s">
@@ -11944,7 +11944,7 @@
       <c r="H9" t="s">
         <v>25</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="2">
         <v>44257</v>
       </c>
       <c r="J9" t="s">
@@ -12003,7 +12003,7 @@
       <c r="H10" t="s">
         <v>25</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="2">
         <v>44375</v>
       </c>
       <c r="J10" t="s">
@@ -12062,7 +12062,7 @@
       <c r="H11" t="s">
         <v>25</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="2">
         <v>37676</v>
       </c>
       <c r="J11" t="s">
@@ -12121,7 +12121,7 @@
       <c r="H12" t="s">
         <v>25</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="2">
         <v>44379</v>
       </c>
       <c r="J12" t="s">
@@ -12180,7 +12180,7 @@
       <c r="H13" t="s">
         <v>25</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="2">
         <v>44494</v>
       </c>
       <c r="J13" t="s">
@@ -12239,7 +12239,7 @@
       <c r="H14" t="s">
         <v>25</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="2">
         <v>44251</v>
       </c>
       <c r="J14" t="s">
@@ -12295,7 +12295,7 @@
       <c r="H15" t="s">
         <v>25</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="2">
         <v>44375</v>
       </c>
       <c r="J15" t="s">
@@ -12354,7 +12354,7 @@
       <c r="H16" t="s">
         <v>25</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="2">
         <v>44247</v>
       </c>
       <c r="J16" t="s">
@@ -12413,7 +12413,7 @@
       <c r="H17" t="s">
         <v>25</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="2">
         <v>44226</v>
       </c>
       <c r="J17" t="s">
@@ -12475,7 +12475,7 @@
       <c r="H18" t="s">
         <v>25</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="2">
         <v>44494</v>
       </c>
       <c r="J18" t="s">
@@ -12537,7 +12537,7 @@
       <c r="H19" t="s">
         <v>25</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="2">
         <v>44226</v>
       </c>
       <c r="J19" t="s">
@@ -12599,7 +12599,7 @@
       <c r="H20" t="s">
         <v>25</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="2">
         <v>44494</v>
       </c>
       <c r="J20" t="s">
@@ -12658,7 +12658,7 @@
       <c r="H21" t="s">
         <v>25</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="2">
         <v>44226</v>
       </c>
       <c r="J21" t="s">
@@ -12714,7 +12714,7 @@
       <c r="H22" t="s">
         <v>25</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="2">
         <v>44375</v>
       </c>
       <c r="J22" t="s">
@@ -12773,7 +12773,7 @@
       <c r="H23" t="s">
         <v>25</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="2">
         <v>41694</v>
       </c>
       <c r="J23" t="s">
@@ -12835,7 +12835,7 @@
       <c r="H24" t="s">
         <v>25</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="2">
         <v>44226</v>
       </c>
       <c r="J24" t="s">
@@ -12897,7 +12897,7 @@
       <c r="H25" t="s">
         <v>25</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="2">
         <v>44226</v>
       </c>
       <c r="J25" t="s">
@@ -12959,7 +12959,7 @@
       <c r="H26" t="s">
         <v>25</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="2">
         <v>44226</v>
       </c>
       <c r="J26" t="s">
@@ -13018,7 +13018,7 @@
       <c r="H27" t="s">
         <v>25</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="2">
         <v>44494</v>
       </c>
       <c r="J27" t="s">
@@ -13074,7 +13074,7 @@
       <c r="H28" t="s">
         <v>25</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="2">
         <v>44375</v>
       </c>
       <c r="J28" t="s">
@@ -13133,7 +13133,7 @@
       <c r="H29" t="s">
         <v>25</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="2">
         <v>44237</v>
       </c>
       <c r="J29" t="s">
@@ -13189,7 +13189,7 @@
       <c r="H30" t="s">
         <v>25</v>
       </c>
-      <c r="I30">
+      <c r="I30" s="2">
         <v>44494</v>
       </c>
       <c r="J30" t="s">
@@ -13248,7 +13248,7 @@
       <c r="H31" t="s">
         <v>25</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="2">
         <v>44501</v>
       </c>
       <c r="J31" t="s">
@@ -13304,7 +13304,7 @@
       <c r="H32" t="s">
         <v>25</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="2">
         <v>44226</v>
       </c>
       <c r="J32" t="s">
@@ -13366,7 +13366,7 @@
       <c r="H33" t="s">
         <v>25</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="2">
         <v>38404</v>
       </c>
       <c r="J33" t="s">
@@ -13428,7 +13428,7 @@
       <c r="H34" t="s">
         <v>25</v>
       </c>
-      <c r="I34">
+      <c r="I34" s="2">
         <v>44226</v>
       </c>
       <c r="J34" t="s">
@@ -13487,7 +13487,7 @@
       <c r="H35" t="s">
         <v>25</v>
       </c>
-      <c r="I35">
+      <c r="I35" s="2">
         <v>43035</v>
       </c>
       <c r="J35" t="s">
@@ -13552,7 +13552,7 @@
       <c r="H36" t="s">
         <v>25</v>
       </c>
-      <c r="I36">
+      <c r="I36" s="2">
         <v>44494</v>
       </c>
       <c r="J36" t="s">
@@ -13611,7 +13611,7 @@
       <c r="H37" t="s">
         <v>25</v>
       </c>
-      <c r="I37">
+      <c r="I37" s="2">
         <v>44496</v>
       </c>
       <c r="J37" t="s">
@@ -13667,7 +13667,7 @@
       <c r="H38" t="s">
         <v>25</v>
       </c>
-      <c r="I38">
+      <c r="I38" s="2">
         <v>44253</v>
       </c>
       <c r="J38" t="s">
@@ -13726,7 +13726,7 @@
       <c r="H39" t="s">
         <v>25</v>
       </c>
-      <c r="I39">
+      <c r="I39" s="2">
         <v>44494</v>
       </c>
       <c r="J39" t="s">
@@ -13785,7 +13785,7 @@
       <c r="H40" t="s">
         <v>25</v>
       </c>
-      <c r="I40">
+      <c r="I40" s="2">
         <v>44263</v>
       </c>
       <c r="J40" t="s">
@@ -13847,7 +13847,7 @@
       <c r="H41" t="s">
         <v>25</v>
       </c>
-      <c r="I41">
+      <c r="I41" s="2">
         <v>44235</v>
       </c>
       <c r="J41" t="s">
@@ -13909,7 +13909,7 @@
       <c r="H42" t="s">
         <v>25</v>
       </c>
-      <c r="I42">
+      <c r="I42" s="2">
         <v>44375</v>
       </c>
       <c r="J42" t="s">
@@ -13965,7 +13965,7 @@
       <c r="H43" t="s">
         <v>25</v>
       </c>
-      <c r="I43">
+      <c r="I43" s="2">
         <v>44226</v>
       </c>
       <c r="J43" t="s">
@@ -14024,7 +14024,7 @@
       <c r="H44" t="s">
         <v>25</v>
       </c>
-      <c r="I44">
+      <c r="I44" s="2">
         <v>44226</v>
       </c>
       <c r="J44" t="s">
@@ -14083,7 +14083,7 @@
       <c r="H45" t="s">
         <v>25</v>
       </c>
-      <c r="I45">
+      <c r="I45" s="2">
         <v>44226</v>
       </c>
       <c r="J45" t="s">
@@ -14145,7 +14145,7 @@
       <c r="H46" t="s">
         <v>25</v>
       </c>
-      <c r="I46">
+      <c r="I46" s="2">
         <v>44226</v>
       </c>
       <c r="J46" t="s">
@@ -14204,7 +14204,7 @@
       <c r="H47" t="s">
         <v>25</v>
       </c>
-      <c r="I47">
+      <c r="I47" s="2">
         <v>44375</v>
       </c>
       <c r="J47" t="s">
@@ -14266,7 +14266,7 @@
       <c r="H48" t="s">
         <v>25</v>
       </c>
-      <c r="I48">
+      <c r="I48" s="2">
         <v>44375</v>
       </c>
       <c r="J48" t="s">
@@ -14328,7 +14328,7 @@
       <c r="H49" t="s">
         <v>25</v>
       </c>
-      <c r="I49">
+      <c r="I49" s="2">
         <v>44247</v>
       </c>
       <c r="J49" t="s">
@@ -14387,7 +14387,7 @@
       <c r="H50" t="s">
         <v>25</v>
       </c>
-      <c r="I50">
+      <c r="I50" s="2">
         <v>44494</v>
       </c>
       <c r="J50" t="s">
@@ -14446,7 +14446,7 @@
       <c r="H51" t="s">
         <v>25</v>
       </c>
-      <c r="I51">
+      <c r="I51" s="2">
         <v>44233</v>
       </c>
       <c r="J51" t="s">
@@ -14505,7 +14505,7 @@
       <c r="H52" t="s">
         <v>25</v>
       </c>
-      <c r="I52">
+      <c r="I52" s="2">
         <v>44130</v>
       </c>
       <c r="J52" t="s">
@@ -14567,7 +14567,7 @@
       <c r="H53" t="s">
         <v>25</v>
       </c>
-      <c r="I53">
+      <c r="I53" s="2">
         <v>44375</v>
       </c>
       <c r="J53" t="s">
@@ -14623,7 +14623,7 @@
       <c r="H54" t="s">
         <v>25</v>
       </c>
-      <c r="I54">
+      <c r="I54" s="2">
         <v>44255</v>
       </c>
       <c r="J54" t="s">
@@ -14679,7 +14679,7 @@
       <c r="H55" t="s">
         <v>25</v>
       </c>
-      <c r="I55">
+      <c r="I55" s="2">
         <v>44249</v>
       </c>
       <c r="J55" t="s">
@@ -14741,7 +14741,7 @@
       <c r="H56" t="s">
         <v>25</v>
       </c>
-      <c r="I56">
+      <c r="I56" s="2">
         <v>44375</v>
       </c>
       <c r="J56" t="s">
@@ -14800,7 +14800,7 @@
       <c r="H57" t="s">
         <v>25</v>
       </c>
-      <c r="I57">
+      <c r="I57" s="2">
         <v>44375</v>
       </c>
       <c r="J57" t="s">
@@ -14859,7 +14859,7 @@
       <c r="H58" t="s">
         <v>25</v>
       </c>
-      <c r="I58">
+      <c r="I58" s="2">
         <v>44226</v>
       </c>
       <c r="J58" t="s">
@@ -14918,7 +14918,7 @@
       <c r="H59" t="s">
         <v>25</v>
       </c>
-      <c r="I59">
+      <c r="I59" s="2">
         <v>44238</v>
       </c>
       <c r="J59" t="s">
@@ -14977,7 +14977,7 @@
       <c r="H60" t="s">
         <v>25</v>
       </c>
-      <c r="I60">
+      <c r="I60" s="2">
         <v>43290</v>
       </c>
       <c r="J60" t="s">
@@ -15039,7 +15039,7 @@
       <c r="H61" t="s">
         <v>25</v>
       </c>
-      <c r="I61">
+      <c r="I61" s="2">
         <v>44375</v>
       </c>
       <c r="J61" t="s">
@@ -15101,7 +15101,7 @@
       <c r="H62" t="s">
         <v>25</v>
       </c>
-      <c r="I62">
+      <c r="I62" s="2">
         <v>44375</v>
       </c>
       <c r="J62" t="s">
@@ -15157,7 +15157,7 @@
       <c r="H63" t="s">
         <v>25</v>
       </c>
-      <c r="I63">
+      <c r="I63" s="2">
         <v>44226</v>
       </c>
       <c r="J63" t="s">
@@ -15216,7 +15216,7 @@
       <c r="H64" t="s">
         <v>25</v>
       </c>
-      <c r="I64">
+      <c r="I64" s="2">
         <v>44494</v>
       </c>
       <c r="J64" t="s">
@@ -15272,7 +15272,7 @@
       <c r="H65" t="s">
         <v>25</v>
       </c>
-      <c r="I65">
+      <c r="I65" s="2">
         <v>44494</v>
       </c>
       <c r="J65" t="s">
@@ -15334,7 +15334,7 @@
       <c r="H66" t="s">
         <v>25</v>
       </c>
-      <c r="I66">
+      <c r="I66" s="2">
         <v>44375</v>
       </c>
       <c r="J66" t="s">
@@ -15393,7 +15393,7 @@
       <c r="H67" t="s">
         <v>25</v>
       </c>
-      <c r="I67">
+      <c r="I67" s="2">
         <v>44494</v>
       </c>
       <c r="J67" t="s">
@@ -15446,7 +15446,7 @@
       <c r="H68" t="s">
         <v>25</v>
       </c>
-      <c r="I68">
+      <c r="I68" s="2">
         <v>44375</v>
       </c>
       <c r="J68" t="s">
@@ -15508,7 +15508,7 @@
       <c r="H69" t="s">
         <v>25</v>
       </c>
-      <c r="I69">
+      <c r="I69" s="2">
         <v>43409</v>
       </c>
       <c r="J69" t="s">
@@ -15570,7 +15570,7 @@
       <c r="H70" t="s">
         <v>25</v>
       </c>
-      <c r="I70">
+      <c r="I70" s="2">
         <v>44238</v>
       </c>
       <c r="J70" t="s">
@@ -15629,7 +15629,7 @@
       <c r="H71" t="s">
         <v>25</v>
       </c>
-      <c r="I71">
+      <c r="I71" s="2">
         <v>40224</v>
       </c>
       <c r="J71" t="s">
@@ -15688,7 +15688,7 @@
       <c r="H72" t="s">
         <v>25</v>
       </c>
-      <c r="I72">
+      <c r="I72" s="2">
         <v>44226</v>
       </c>
       <c r="J72" t="s">
@@ -15744,7 +15744,7 @@
       <c r="H73" t="s">
         <v>25</v>
       </c>
-      <c r="I73">
+      <c r="I73" s="2">
         <v>44226</v>
       </c>
       <c r="J73" t="s">
@@ -15803,7 +15803,7 @@
       <c r="H74" t="s">
         <v>25</v>
       </c>
-      <c r="I74">
+      <c r="I74" s="2">
         <v>44226</v>
       </c>
       <c r="J74" t="s">
@@ -15862,7 +15862,7 @@
       <c r="H75" t="s">
         <v>25</v>
       </c>
-      <c r="I75">
+      <c r="I75" s="2">
         <v>44226</v>
       </c>
       <c r="J75" t="s">
@@ -15921,7 +15921,7 @@
       <c r="H76" t="s">
         <v>25</v>
       </c>
-      <c r="I76">
+      <c r="I76" s="2">
         <v>44253</v>
       </c>
       <c r="J76" t="s">
@@ -15977,7 +15977,7 @@
       <c r="H77" t="s">
         <v>25</v>
       </c>
-      <c r="I77">
+      <c r="I77" s="2">
         <v>39125</v>
       </c>
       <c r="J77" t="s">
@@ -16039,7 +16039,7 @@
       <c r="H78" t="s">
         <v>25</v>
       </c>
-      <c r="I78">
+      <c r="I78" s="2">
         <v>44233</v>
       </c>
       <c r="J78" t="s">
@@ -16098,7 +16098,7 @@
       <c r="H79" t="s">
         <v>25</v>
       </c>
-      <c r="I79">
+      <c r="I79" s="2">
         <v>44226</v>
       </c>
       <c r="J79" t="s">
@@ -16157,7 +16157,7 @@
       <c r="H80" t="s">
         <v>25</v>
       </c>
-      <c r="I80">
+      <c r="I80" s="2">
         <v>44226</v>
       </c>
       <c r="J80" t="s">
@@ -16219,7 +16219,7 @@
       <c r="H81" t="s">
         <v>25</v>
       </c>
-      <c r="I81">
+      <c r="I81" s="2">
         <v>44226</v>
       </c>
       <c r="J81" t="s">
@@ -16278,7 +16278,7 @@
       <c r="H82" t="s">
         <v>25</v>
       </c>
-      <c r="I82">
+      <c r="I82" s="2">
         <v>44226</v>
       </c>
       <c r="J82" t="s">
@@ -16337,7 +16337,7 @@
       <c r="H83" t="s">
         <v>25</v>
       </c>
-      <c r="I83">
+      <c r="I83" s="2">
         <v>44226</v>
       </c>
       <c r="J83" t="s">
@@ -16396,7 +16396,7 @@
       <c r="H84" t="s">
         <v>25</v>
       </c>
-      <c r="I84">
+      <c r="I84" s="2">
         <v>44494</v>
       </c>
       <c r="J84" t="s">
@@ -16455,7 +16455,7 @@
       <c r="H85" t="s">
         <v>25</v>
       </c>
-      <c r="I85">
+      <c r="I85" s="2">
         <v>44239</v>
       </c>
       <c r="J85" t="s">
@@ -16517,7 +16517,7 @@
       <c r="H86" t="s">
         <v>25</v>
       </c>
-      <c r="I86">
+      <c r="I86" s="2">
         <v>44239</v>
       </c>
       <c r="J86" t="s">
@@ -16579,7 +16579,7 @@
       <c r="H87" t="s">
         <v>25</v>
       </c>
-      <c r="I87">
+      <c r="I87" s="2">
         <v>42786</v>
       </c>
       <c r="J87" t="s">
@@ -16641,7 +16641,7 @@
       <c r="H88" t="s">
         <v>25</v>
       </c>
-      <c r="I88">
+      <c r="I88" s="2">
         <v>44375</v>
       </c>
       <c r="J88" t="s">
@@ -16700,7 +16700,7 @@
       <c r="H89" t="s">
         <v>25</v>
       </c>
-      <c r="I89">
+      <c r="I89" s="2">
         <v>44246</v>
       </c>
       <c r="J89" t="s">
@@ -16759,7 +16759,7 @@
       <c r="H90" t="s">
         <v>25</v>
       </c>
-      <c r="I90">
+      <c r="I90" s="2">
         <v>41330</v>
       </c>
       <c r="J90" t="s">
@@ -16821,7 +16821,7 @@
       <c r="H91" t="s">
         <v>25</v>
       </c>
-      <c r="I91">
+      <c r="I91" s="2">
         <v>44226</v>
       </c>
       <c r="J91" t="s">
@@ -16883,7 +16883,7 @@
       <c r="H92" t="s">
         <v>25</v>
       </c>
-      <c r="I92">
+      <c r="I92" s="2">
         <v>44253</v>
       </c>
       <c r="J92" t="s">
@@ -16945,7 +16945,7 @@
       <c r="H93" t="s">
         <v>25</v>
       </c>
-      <c r="I93">
+      <c r="I93" s="2">
         <v>44230</v>
       </c>
       <c r="J93" t="s">
@@ -17007,7 +17007,7 @@
       <c r="H94" t="s">
         <v>25</v>
       </c>
-      <c r="I94">
+      <c r="I94" s="2">
         <v>44226</v>
       </c>
       <c r="J94" t="s">
@@ -17066,7 +17066,7 @@
       <c r="H95" t="s">
         <v>25</v>
       </c>
-      <c r="I95">
+      <c r="I95" s="2">
         <v>42310</v>
       </c>
       <c r="J95" t="s">
@@ -17122,7 +17122,7 @@
       <c r="H96" t="s">
         <v>25</v>
       </c>
-      <c r="I96">
+      <c r="I96" s="2">
         <v>44226</v>
       </c>
       <c r="J96" t="s">
@@ -17184,7 +17184,7 @@
       <c r="H97" t="s">
         <v>25</v>
       </c>
-      <c r="I97">
+      <c r="I97" s="2">
         <v>44226</v>
       </c>
       <c r="J97" t="s">
@@ -17243,7 +17243,7 @@
       <c r="H98" t="s">
         <v>25</v>
       </c>
-      <c r="I98">
+      <c r="I98" s="2">
         <v>44375</v>
       </c>
       <c r="J98" t="s">
@@ -17305,7 +17305,7 @@
       <c r="H99" t="s">
         <v>25</v>
       </c>
-      <c r="I99">
+      <c r="I99" s="2">
         <v>44494</v>
       </c>
       <c r="J99" t="s">
@@ -17367,7 +17367,7 @@
       <c r="H100" t="s">
         <v>25</v>
       </c>
-      <c r="I100">
+      <c r="I100" s="2">
         <v>44494</v>
       </c>
       <c r="J100" t="s">
@@ -17426,7 +17426,7 @@
       <c r="H101" t="s">
         <v>25</v>
       </c>
-      <c r="I101">
+      <c r="I101" s="2">
         <v>44238</v>
       </c>
       <c r="J101" t="s">
@@ -17488,7 +17488,7 @@
       <c r="H102" t="s">
         <v>25</v>
       </c>
-      <c r="I102">
+      <c r="I102" s="2">
         <v>44249</v>
       </c>
       <c r="J102" t="s">
@@ -17550,7 +17550,7 @@
       <c r="H103" t="s">
         <v>25</v>
       </c>
-      <c r="I103">
+      <c r="I103" s="2">
         <v>44379</v>
       </c>
       <c r="J103" t="s">
@@ -17609,7 +17609,7 @@
       <c r="H104" t="s">
         <v>25</v>
       </c>
-      <c r="I104">
+      <c r="I104" s="2">
         <v>44375</v>
       </c>
       <c r="J104" t="s">
@@ -17668,7 +17668,7 @@
       <c r="H105" t="s">
         <v>25</v>
       </c>
-      <c r="I105">
+      <c r="I105" s="2">
         <v>44226</v>
       </c>
       <c r="J105" t="s">
@@ -17727,7 +17727,7 @@
       <c r="H106" t="s">
         <v>25</v>
       </c>
-      <c r="I106">
+      <c r="I106" s="2">
         <v>44252</v>
       </c>
       <c r="J106" t="s">
@@ -17786,7 +17786,7 @@
       <c r="H107" t="s">
         <v>25</v>
       </c>
-      <c r="I107">
+      <c r="I107" s="2">
         <v>44226</v>
       </c>
       <c r="J107" t="s">
@@ -17845,7 +17845,7 @@
       <c r="H108" t="s">
         <v>25</v>
       </c>
-      <c r="I108">
+      <c r="I108" s="2">
         <v>44226</v>
       </c>
       <c r="J108" t="s">
@@ -17901,7 +17901,7 @@
       <c r="H109" t="s">
         <v>25</v>
       </c>
-      <c r="I109">
+      <c r="I109" s="2">
         <v>44375</v>
       </c>
       <c r="J109" t="s">
@@ -17963,7 +17963,7 @@
       <c r="H110" t="s">
         <v>25</v>
       </c>
-      <c r="I110">
+      <c r="I110" s="2">
         <v>44228</v>
       </c>
       <c r="J110" t="s">
@@ -18019,7 +18019,7 @@
       <c r="H111" t="s">
         <v>25</v>
       </c>
-      <c r="I111">
+      <c r="I111" s="2">
         <v>43031</v>
       </c>
       <c r="J111" t="s">
@@ -18075,7 +18075,7 @@
       <c r="H112" t="s">
         <v>25</v>
       </c>
-      <c r="I112">
+      <c r="I112" s="2">
         <v>44375</v>
       </c>
       <c r="J112" t="s">
@@ -18131,7 +18131,7 @@
       <c r="H113" t="s">
         <v>25</v>
       </c>
-      <c r="I113">
+      <c r="I113" s="2">
         <v>42786</v>
       </c>
       <c r="J113" t="s">
@@ -18193,7 +18193,7 @@
       <c r="H114" t="s">
         <v>25</v>
       </c>
-      <c r="I114">
+      <c r="I114" s="2">
         <v>44375</v>
       </c>
       <c r="J114" t="s">
@@ -18249,7 +18249,7 @@
       <c r="H115" t="s">
         <v>25</v>
       </c>
-      <c r="I115">
+      <c r="I115" s="2">
         <v>44226</v>
       </c>
       <c r="J115" t="s">
@@ -18308,7 +18308,7 @@
       <c r="H116" t="s">
         <v>25</v>
       </c>
-      <c r="I116">
+      <c r="I116" s="2">
         <v>44375</v>
       </c>
       <c r="J116" t="s">
@@ -18370,7 +18370,7 @@
       <c r="H117" t="s">
         <v>25</v>
       </c>
-      <c r="I117">
+      <c r="I117" s="2">
         <v>36941</v>
       </c>
       <c r="J117" t="s">
@@ -18432,7 +18432,7 @@
       <c r="H118" t="s">
         <v>25</v>
       </c>
-      <c r="I118">
+      <c r="I118" s="2">
         <v>44226</v>
       </c>
       <c r="J118" t="s">
@@ -18491,7 +18491,7 @@
       <c r="H119" t="s">
         <v>25</v>
       </c>
-      <c r="I119">
+      <c r="I119" s="2">
         <v>42786</v>
       </c>
       <c r="J119" t="s">
@@ -18550,7 +18550,7 @@
       <c r="H120" t="s">
         <v>25</v>
       </c>
-      <c r="I120">
+      <c r="I120" s="2">
         <v>44226</v>
       </c>
       <c r="J120" t="s">
@@ -18612,7 +18612,7 @@
       <c r="H121" t="s">
         <v>25</v>
       </c>
-      <c r="I121">
+      <c r="I121" s="2">
         <v>43290</v>
       </c>
       <c r="J121" t="s">
@@ -18674,7 +18674,7 @@
       <c r="H122" t="s">
         <v>25</v>
       </c>
-      <c r="I122">
+      <c r="I122" s="2">
         <v>43409</v>
       </c>
       <c r="J122" t="s">
@@ -18736,7 +18736,7 @@
       <c r="H123" t="s">
         <v>25</v>
       </c>
-      <c r="I123">
+      <c r="I123" s="2">
         <v>44501</v>
       </c>
       <c r="J123" t="s">
@@ -18798,7 +18798,7 @@
       <c r="H124" t="s">
         <v>25</v>
       </c>
-      <c r="I124">
+      <c r="I124" s="2">
         <v>43773</v>
       </c>
       <c r="J124" t="s">
@@ -18860,7 +18860,7 @@
       <c r="H125" t="s">
         <v>25</v>
       </c>
-      <c r="I125">
+      <c r="I125" s="2">
         <v>44226</v>
       </c>
       <c r="J125" t="s">
@@ -18922,7 +18922,7 @@
       <c r="H126" t="s">
         <v>25</v>
       </c>
-      <c r="I126">
+      <c r="I126" s="2">
         <v>44226</v>
       </c>
       <c r="J126" t="s">
@@ -18981,7 +18981,7 @@
       <c r="H127" t="s">
         <v>25</v>
       </c>
-      <c r="I127">
+      <c r="I127" s="2">
         <v>44494</v>
       </c>
       <c r="J127" t="s">
@@ -19043,7 +19043,7 @@
       <c r="H128" t="s">
         <v>25</v>
       </c>
-      <c r="I128">
+      <c r="I128" s="2">
         <v>44494</v>
       </c>
       <c r="J128" t="s">
@@ -19102,7 +19102,7 @@
       <c r="H129" t="s">
         <v>25</v>
       </c>
-      <c r="I129">
+      <c r="I129" s="2">
         <v>44494</v>
       </c>
       <c r="J129" t="s">
@@ -19164,7 +19164,7 @@
       <c r="H130" t="s">
         <v>25</v>
       </c>
-      <c r="I130">
+      <c r="I130" s="2">
         <v>44494</v>
       </c>
       <c r="J130" t="s">
@@ -19223,7 +19223,7 @@
       <c r="H131" t="s">
         <v>25</v>
       </c>
-      <c r="I131">
+      <c r="I131" s="2">
         <v>44261</v>
       </c>
       <c r="J131" t="s">
@@ -19282,7 +19282,7 @@
       <c r="H132" t="s">
         <v>25</v>
       </c>
-      <c r="I132">
+      <c r="I132" s="2">
         <v>44375</v>
       </c>
       <c r="J132" t="s">
@@ -19341,7 +19341,7 @@
       <c r="H133" t="s">
         <v>25</v>
       </c>
-      <c r="I133">
+      <c r="I133" s="2">
         <v>44226</v>
       </c>
       <c r="J133" t="s">
@@ -19400,7 +19400,7 @@
       <c r="H134" t="s">
         <v>25</v>
       </c>
-      <c r="I134">
+      <c r="I134" s="2">
         <v>44263</v>
       </c>
       <c r="J134" t="s">
@@ -19459,7 +19459,7 @@
       <c r="H135" t="s">
         <v>25</v>
       </c>
-      <c r="I135">
+      <c r="I135" s="2">
         <v>44375</v>
       </c>
       <c r="J135" t="s">
@@ -19518,7 +19518,7 @@
       <c r="H136" t="s">
         <v>25</v>
       </c>
-      <c r="I136">
+      <c r="I136" s="2">
         <v>44226</v>
       </c>
       <c r="J136" t="s">
@@ -19577,7 +19577,7 @@
       <c r="H137" t="s">
         <v>25</v>
       </c>
-      <c r="I137">
+      <c r="I137" s="2">
         <v>44494</v>
       </c>
       <c r="J137" t="s">
@@ -19639,7 +19639,7 @@
       <c r="H138" t="s">
         <v>25</v>
       </c>
-      <c r="I138">
+      <c r="I138" s="2">
         <v>43865</v>
       </c>
       <c r="J138" t="s">
@@ -19701,7 +19701,7 @@
       <c r="H139" t="s">
         <v>25</v>
       </c>
-      <c r="I139">
+      <c r="I139" s="2">
         <v>44501</v>
       </c>
       <c r="J139" t="s">
@@ -19763,7 +19763,7 @@
       <c r="H140" t="s">
         <v>25</v>
       </c>
-      <c r="I140">
+      <c r="I140" s="2">
         <v>44494</v>
       </c>
       <c r="J140" t="s">
@@ -19825,7 +19825,7 @@
       <c r="H141" t="s">
         <v>25</v>
       </c>
-      <c r="I141">
+      <c r="I141" s="2">
         <v>44226</v>
       </c>
       <c r="J141" t="s">
@@ -19884,7 +19884,7 @@
       <c r="H142" t="s">
         <v>25</v>
       </c>
-      <c r="I142">
+      <c r="I142" s="2">
         <v>44375</v>
       </c>
       <c r="J142" t="s">
@@ -19946,7 +19946,7 @@
       <c r="H143" t="s">
         <v>25</v>
       </c>
-      <c r="I143">
+      <c r="I143" s="2">
         <v>44252</v>
       </c>
       <c r="J143" t="s">
@@ -20005,7 +20005,7 @@
       <c r="H144" t="s">
         <v>25</v>
       </c>
-      <c r="I144">
+      <c r="I144" s="2">
         <v>44375</v>
       </c>
       <c r="J144" t="s">
@@ -20064,7 +20064,7 @@
       <c r="H145" t="s">
         <v>25</v>
       </c>
-      <c r="I145">
+      <c r="I145" s="2">
         <v>42422</v>
       </c>
       <c r="J145" t="s">
@@ -20123,7 +20123,7 @@
       <c r="H146" t="s">
         <v>25</v>
       </c>
-      <c r="I146">
+      <c r="I146" s="2">
         <v>44226</v>
       </c>
       <c r="J146" t="s">
@@ -20182,7 +20182,7 @@
       <c r="H147" t="s">
         <v>25</v>
       </c>
-      <c r="I147">
+      <c r="I147" s="2">
         <v>44375</v>
       </c>
       <c r="J147" t="s">
@@ -20244,7 +20244,7 @@
       <c r="H148" t="s">
         <v>25</v>
       </c>
-      <c r="I148">
+      <c r="I148" s="2">
         <v>44494</v>
       </c>
       <c r="J148" t="s">
@@ -20303,7 +20303,7 @@
       <c r="H149" t="s">
         <v>25</v>
       </c>
-      <c r="I149">
+      <c r="I149" s="2">
         <v>44130</v>
       </c>
       <c r="J149" t="s">
@@ -20362,7 +20362,7 @@
       <c r="H150" t="s">
         <v>25</v>
       </c>
-      <c r="I150">
+      <c r="I150" s="2">
         <v>44494</v>
       </c>
       <c r="J150" t="s">
@@ -20418,7 +20418,7 @@
       <c r="H151" t="s">
         <v>25</v>
       </c>
-      <c r="I151">
+      <c r="I151" s="2">
         <v>44494</v>
       </c>
       <c r="J151" t="s">
@@ -20474,7 +20474,7 @@
       <c r="H152" t="s">
         <v>25</v>
       </c>
-      <c r="I152">
+      <c r="I152" s="2">
         <v>44375</v>
       </c>
       <c r="J152" t="s">
@@ -20536,7 +20536,7 @@
       <c r="H153" t="s">
         <v>25</v>
       </c>
-      <c r="I153">
+      <c r="I153" s="2">
         <v>44376</v>
       </c>
       <c r="J153" t="s">
@@ -20592,7 +20592,7 @@
       <c r="H154" t="s">
         <v>25</v>
       </c>
-      <c r="I154">
+      <c r="I154" s="2">
         <v>44226</v>
       </c>
       <c r="J154" t="s">
@@ -20651,7 +20651,7 @@
       <c r="H155" t="s">
         <v>25</v>
       </c>
-      <c r="I155">
+      <c r="I155" s="2">
         <v>44226</v>
       </c>
       <c r="J155" t="s">
@@ -20713,7 +20713,7 @@
       <c r="H156" t="s">
         <v>25</v>
       </c>
-      <c r="I156">
+      <c r="I156" s="2">
         <v>44494</v>
       </c>
       <c r="J156" t="s">
@@ -20769,7 +20769,7 @@
       <c r="H157" t="s">
         <v>25</v>
       </c>
-      <c r="I157">
+      <c r="I157" s="2">
         <v>44494</v>
       </c>
       <c r="J157" t="s">
@@ -20828,7 +20828,7 @@
       <c r="H158" t="s">
         <v>25</v>
       </c>
-      <c r="I158">
+      <c r="I158" s="2">
         <v>44375</v>
       </c>
       <c r="J158" t="s">
@@ -20890,7 +20890,7 @@
       <c r="H159" t="s">
         <v>25</v>
       </c>
-      <c r="I159">
+      <c r="I159" s="2">
         <v>44226</v>
       </c>
       <c r="J159" t="s">
@@ -20946,7 +20946,7 @@
       <c r="H160" t="s">
         <v>25</v>
       </c>
-      <c r="I160">
+      <c r="I160" s="2">
         <v>44375</v>
       </c>
       <c r="J160" t="s">
@@ -21008,7 +21008,7 @@
       <c r="H161" t="s">
         <v>25</v>
       </c>
-      <c r="I161">
+      <c r="I161" s="2">
         <v>44248</v>
       </c>
       <c r="J161" t="s">
@@ -21064,7 +21064,7 @@
       <c r="H162" t="s">
         <v>25</v>
       </c>
-      <c r="I162">
+      <c r="I162" s="2">
         <v>41211</v>
       </c>
       <c r="J162" t="s">
@@ -21126,7 +21126,7 @@
       <c r="H163" t="s">
         <v>25</v>
       </c>
-      <c r="I163">
+      <c r="I163" s="2">
         <v>44232</v>
       </c>
       <c r="J163" t="s">
@@ -21182,7 +21182,7 @@
       <c r="H164" t="s">
         <v>25</v>
       </c>
-      <c r="I164">
+      <c r="I164" s="2">
         <v>41085</v>
       </c>
       <c r="J164" t="s">
@@ -21241,7 +21241,7 @@
       <c r="H165" t="s">
         <v>25</v>
       </c>
-      <c r="I165">
+      <c r="I165" s="2">
         <v>44226</v>
       </c>
       <c r="J165" t="s">
@@ -21300,7 +21300,7 @@
       <c r="H166" t="s">
         <v>25</v>
       </c>
-      <c r="I166">
+      <c r="I166" s="2">
         <v>43654</v>
       </c>
       <c r="J166" t="s">
@@ -21362,7 +21362,7 @@
       <c r="H167" t="s">
         <v>25</v>
       </c>
-      <c r="I167">
+      <c r="I167" s="2">
         <v>44226</v>
       </c>
       <c r="J167" t="s">
@@ -21421,7 +21421,7 @@
       <c r="H168" t="s">
         <v>25</v>
       </c>
-      <c r="I168">
+      <c r="I168" s="2">
         <v>44375</v>
       </c>
       <c r="J168" t="s">
@@ -21483,7 +21483,7 @@
       <c r="H169" t="s">
         <v>25</v>
       </c>
-      <c r="I169">
+      <c r="I169" s="2">
         <v>44375</v>
       </c>
       <c r="J169" t="s">
@@ -21545,7 +21545,7 @@
       <c r="H170" t="s">
         <v>25</v>
       </c>
-      <c r="I170">
+      <c r="I170" s="2">
         <v>44375</v>
       </c>
       <c r="J170" t="s">
@@ -21601,7 +21601,7 @@
       <c r="H171" t="s">
         <v>25</v>
       </c>
-      <c r="I171">
+      <c r="I171" s="2">
         <v>44235</v>
       </c>
       <c r="J171" t="s">
@@ -21660,7 +21660,7 @@
       <c r="H172" t="s">
         <v>25</v>
       </c>
-      <c r="I172">
+      <c r="I172" s="2">
         <v>44494</v>
       </c>
       <c r="J172" t="s">
@@ -21719,7 +21719,7 @@
       <c r="H173" t="s">
         <v>25</v>
       </c>
-      <c r="I173">
+      <c r="I173" s="2">
         <v>44494</v>
       </c>
       <c r="J173" t="s">
@@ -21775,7 +21775,7 @@
       <c r="H174" t="s">
         <v>25</v>
       </c>
-      <c r="I174">
+      <c r="I174" s="2">
         <v>44375</v>
       </c>
       <c r="J174" t="s">
@@ -21834,7 +21834,7 @@
       <c r="H175" t="s">
         <v>25</v>
       </c>
-      <c r="I175">
+      <c r="I175" s="2">
         <v>42422</v>
       </c>
       <c r="J175" t="s">
@@ -21893,7 +21893,7 @@
       <c r="H176" t="s">
         <v>25</v>
       </c>
-      <c r="I176">
+      <c r="I176" s="2">
         <v>44253</v>
       </c>
       <c r="J176" t="s">
@@ -21946,7 +21946,7 @@
       <c r="H177" t="s">
         <v>25</v>
       </c>
-      <c r="I177">
+      <c r="I177" s="2">
         <v>44226</v>
       </c>
       <c r="J177" t="s">
@@ -22005,7 +22005,7 @@
       <c r="H178" t="s">
         <v>25</v>
       </c>
-      <c r="I178">
+      <c r="I178" s="2">
         <v>44375</v>
       </c>
       <c r="J178" t="s">
@@ -22067,7 +22067,7 @@
       <c r="H179" t="s">
         <v>25</v>
       </c>
-      <c r="I179">
+      <c r="I179" s="2">
         <v>44226</v>
       </c>
       <c r="J179" t="s">
@@ -22126,7 +22126,7 @@
       <c r="H180" t="s">
         <v>25</v>
       </c>
-      <c r="I180">
+      <c r="I180" s="2">
         <v>44375</v>
       </c>
       <c r="J180" t="s">
@@ -22179,7 +22179,7 @@
       <c r="H181" t="s">
         <v>25</v>
       </c>
-      <c r="I181">
+      <c r="I181" s="2">
         <v>44238</v>
       </c>
       <c r="J181" t="s">
@@ -22235,7 +22235,7 @@
       <c r="H182" t="s">
         <v>25</v>
       </c>
-      <c r="I182">
+      <c r="I182" s="2">
         <v>44494</v>
       </c>
       <c r="J182" t="s">
@@ -22294,7 +22294,7 @@
       <c r="H183" t="s">
         <v>25</v>
       </c>
-      <c r="I183">
+      <c r="I183" s="2">
         <v>42184</v>
       </c>
       <c r="J183" t="s">
@@ -22356,7 +22356,7 @@
       <c r="H184" t="s">
         <v>25</v>
       </c>
-      <c r="I184">
+      <c r="I184" s="2">
         <v>44494</v>
       </c>
       <c r="J184" t="s">
@@ -22415,7 +22415,7 @@
       <c r="H185" t="s">
         <v>25</v>
       </c>
-      <c r="I185">
+      <c r="I185" s="2">
         <v>44226</v>
       </c>
       <c r="J185" t="s">
@@ -22477,7 +22477,7 @@
       <c r="H186" t="s">
         <v>25</v>
       </c>
-      <c r="I186">
+      <c r="I186" s="2">
         <v>44226</v>
       </c>
       <c r="J186" t="s">
@@ -22539,7 +22539,7 @@
       <c r="H187" t="s">
         <v>25</v>
       </c>
-      <c r="I187">
+      <c r="I187" s="2">
         <v>44494</v>
       </c>
       <c r="J187" t="s">
@@ -22598,7 +22598,7 @@
       <c r="H188" t="s">
         <v>25</v>
       </c>
-      <c r="I188">
+      <c r="I188" s="2">
         <v>44495</v>
       </c>
       <c r="J188" t="s">
@@ -22654,7 +22654,7 @@
       <c r="H189" t="s">
         <v>25</v>
       </c>
-      <c r="I189">
+      <c r="I189" s="2">
         <v>44253</v>
       </c>
       <c r="J189" t="s">
@@ -22713,7 +22713,7 @@
       <c r="H190" t="s">
         <v>25</v>
       </c>
-      <c r="I190">
+      <c r="I190" s="2">
         <v>44252</v>
       </c>
       <c r="J190" t="s">
@@ -22772,7 +22772,7 @@
       <c r="H191" t="s">
         <v>25</v>
       </c>
-      <c r="I191">
+      <c r="I191" s="2">
         <v>44226</v>
       </c>
       <c r="J191" t="s">
@@ -22831,7 +22831,7 @@
       <c r="H192" t="s">
         <v>25</v>
       </c>
-      <c r="I192">
+      <c r="I192" s="2">
         <v>44494</v>
       </c>
       <c r="J192" t="s">
@@ -22893,7 +22893,7 @@
       <c r="H193" t="s">
         <v>25</v>
       </c>
-      <c r="I193">
+      <c r="I193" s="2">
         <v>43164</v>
       </c>
       <c r="J193" t="s">
@@ -22952,7 +22952,7 @@
       <c r="H194" t="s">
         <v>25</v>
       </c>
-      <c r="I194">
+      <c r="I194" s="2">
         <v>44501</v>
       </c>
       <c r="J194" t="s">
@@ -23011,7 +23011,7 @@
       <c r="H195" t="s">
         <v>25</v>
       </c>
-      <c r="I195">
+      <c r="I195" s="2">
         <v>44243</v>
       </c>
       <c r="J195" t="s">
@@ -23067,7 +23067,7 @@
       <c r="H196" t="s">
         <v>25</v>
       </c>
-      <c r="I196">
+      <c r="I196" s="2">
         <v>44375</v>
       </c>
       <c r="J196" t="s">
@@ -23129,7 +23129,7 @@
       <c r="H197" t="s">
         <v>25</v>
       </c>
-      <c r="I197">
+      <c r="I197" s="2">
         <v>44375</v>
       </c>
       <c r="J197" t="s">
@@ -23188,7 +23188,7 @@
       <c r="H198" t="s">
         <v>25</v>
       </c>
-      <c r="I198">
+      <c r="I198" s="2">
         <v>44226</v>
       </c>
       <c r="J198" t="s">
@@ -23247,7 +23247,7 @@
       <c r="H199" t="s">
         <v>25</v>
       </c>
-      <c r="I199">
+      <c r="I199" s="2">
         <v>44377</v>
       </c>
       <c r="J199" t="s">
@@ -23309,7 +23309,7 @@
       <c r="H200" t="s">
         <v>25</v>
       </c>
-      <c r="I200">
+      <c r="I200" s="2">
         <v>40224</v>
       </c>
       <c r="J200" t="s">
@@ -23371,7 +23371,7 @@
       <c r="H201" t="s">
         <v>25</v>
       </c>
-      <c r="I201">
+      <c r="I201" s="2">
         <v>44375</v>
       </c>
       <c r="J201" t="s">
@@ -23433,7 +23433,7 @@
       <c r="H202" t="s">
         <v>25</v>
       </c>
-      <c r="I202">
+      <c r="I202" s="2">
         <v>44255</v>
       </c>
       <c r="J202" t="s">
@@ -23489,7 +23489,7 @@
       <c r="H203" t="s">
         <v>25</v>
       </c>
-      <c r="I203">
+      <c r="I203" s="2">
         <v>44239</v>
       </c>
       <c r="J203" t="s">
@@ -23548,7 +23548,7 @@
       <c r="H204" t="s">
         <v>25</v>
       </c>
-      <c r="I204">
+      <c r="I204" s="2">
         <v>44245</v>
       </c>
       <c r="J204" t="s">
@@ -23607,7 +23607,7 @@
       <c r="H205" t="s">
         <v>25</v>
       </c>
-      <c r="I205">
+      <c r="I205" s="2">
         <v>44226</v>
       </c>
       <c r="J205" t="s">
@@ -23669,7 +23669,7 @@
       <c r="H206" t="s">
         <v>25</v>
       </c>
-      <c r="I206">
+      <c r="I206" s="2">
         <v>44252</v>
       </c>
       <c r="J206" t="s">
@@ -23722,7 +23722,7 @@
       <c r="H207" t="s">
         <v>25</v>
       </c>
-      <c r="I207">
+      <c r="I207" s="2">
         <v>44375</v>
       </c>
       <c r="J207" t="s">
@@ -23778,7 +23778,7 @@
       <c r="H208" t="s">
         <v>25</v>
       </c>
-      <c r="I208">
+      <c r="I208" s="2">
         <v>44375</v>
       </c>
       <c r="J208" t="s">
@@ -23840,7 +23840,7 @@
       <c r="H209" t="s">
         <v>25</v>
       </c>
-      <c r="I209">
+      <c r="I209" s="2">
         <v>44240</v>
       </c>
       <c r="J209" t="s">
@@ -23902,7 +23902,7 @@
       <c r="H210" t="s">
         <v>25</v>
       </c>
-      <c r="I210">
+      <c r="I210" s="2">
         <v>44252</v>
       </c>
       <c r="J210" t="s">
@@ -23955,7 +23955,7 @@
       <c r="H211" t="s">
         <v>25</v>
       </c>
-      <c r="I211">
+      <c r="I211" s="2">
         <v>44494</v>
       </c>
       <c r="J211" t="s">
@@ -24017,7 +24017,7 @@
       <c r="H212" t="s">
         <v>25</v>
       </c>
-      <c r="I212">
+      <c r="I212" s="2">
         <v>44252</v>
       </c>
       <c r="J212" t="s">
@@ -24076,7 +24076,7 @@
       <c r="H213" t="s">
         <v>25</v>
       </c>
-      <c r="I213">
+      <c r="I213" s="2">
         <v>44375</v>
       </c>
       <c r="J213" t="s">
@@ -24138,7 +24138,7 @@
       <c r="H214" t="s">
         <v>25</v>
       </c>
-      <c r="I214">
+      <c r="I214" s="2">
         <v>44494</v>
       </c>
       <c r="J214" t="s">
@@ -24200,7 +24200,7 @@
       <c r="H215" t="s">
         <v>25</v>
       </c>
-      <c r="I215">
+      <c r="I215" s="2">
         <v>44379</v>
       </c>
       <c r="J215" t="s">
@@ -24253,7 +24253,7 @@
       <c r="H216" t="s">
         <v>25</v>
       </c>
-      <c r="I216">
+      <c r="I216" s="2">
         <v>44226</v>
       </c>
       <c r="J216" t="s">
@@ -24309,7 +24309,7 @@
       <c r="H217" t="s">
         <v>25</v>
       </c>
-      <c r="I217">
+      <c r="I217" s="2">
         <v>44226</v>
       </c>
       <c r="J217" t="s">
@@ -24371,7 +24371,7 @@
       <c r="H218" t="s">
         <v>25</v>
       </c>
-      <c r="I218">
+      <c r="I218" s="2">
         <v>44237</v>
       </c>
       <c r="J218" t="s">
@@ -24430,7 +24430,7 @@
       <c r="H219" t="s">
         <v>25</v>
       </c>
-      <c r="I219">
+      <c r="I219" s="2">
         <v>44226</v>
       </c>
       <c r="J219" t="s">
@@ -24489,7 +24489,7 @@
       <c r="H220" t="s">
         <v>25</v>
       </c>
-      <c r="I220">
+      <c r="I220" s="2">
         <v>44226</v>
       </c>
       <c r="J220" t="s">
@@ -24548,7 +24548,7 @@
       <c r="H221" t="s">
         <v>25</v>
       </c>
-      <c r="I221">
+      <c r="I221" s="2">
         <v>44375</v>
       </c>
       <c r="J221" t="s">
@@ -24607,7 +24607,7 @@
       <c r="H222" t="s">
         <v>25</v>
       </c>
-      <c r="I222">
+      <c r="I222" s="2">
         <v>44375</v>
       </c>
       <c r="J222" t="s">
@@ -24666,7 +24666,7 @@
       <c r="H223" t="s">
         <v>25</v>
       </c>
-      <c r="I223">
+      <c r="I223" s="2">
         <v>44237</v>
       </c>
       <c r="J223" t="s">
@@ -24725,7 +24725,7 @@
       <c r="H224" t="s">
         <v>25</v>
       </c>
-      <c r="I224">
+      <c r="I224" s="2">
         <v>44375</v>
       </c>
       <c r="J224" t="s">
@@ -24778,7 +24778,7 @@
       <c r="H225" t="s">
         <v>25</v>
       </c>
-      <c r="I225">
+      <c r="I225" s="2">
         <v>44226</v>
       </c>
       <c r="J225" t="s">
@@ -24837,7 +24837,7 @@
       <c r="H226" t="s">
         <v>25</v>
       </c>
-      <c r="I226">
+      <c r="I226" s="2">
         <v>44226</v>
       </c>
       <c r="J226" t="s">
@@ -24896,7 +24896,7 @@
       <c r="H227" t="s">
         <v>25</v>
       </c>
-      <c r="I227">
+      <c r="I227" s="2">
         <v>44494</v>
       </c>
       <c r="J227" t="s">
@@ -24955,7 +24955,7 @@
       <c r="H228" t="s">
         <v>25</v>
       </c>
-      <c r="I228">
+      <c r="I228" s="2">
         <v>44226</v>
       </c>
       <c r="J228" t="s">
@@ -25011,7 +25011,7 @@
       <c r="H229" t="s">
         <v>25</v>
       </c>
-      <c r="I229">
+      <c r="I229" s="2">
         <v>44242</v>
       </c>
       <c r="J229" t="s">
@@ -25070,7 +25070,7 @@
       <c r="H230" t="s">
         <v>25</v>
       </c>
-      <c r="I230">
+      <c r="I230" s="2">
         <v>44494</v>
       </c>
       <c r="J230" t="s">
@@ -25129,7 +25129,7 @@
       <c r="H231" t="s">
         <v>25</v>
       </c>
-      <c r="I231">
+      <c r="I231" s="2">
         <v>44375</v>
       </c>
       <c r="J231" t="s">
@@ -25185,7 +25185,7 @@
       <c r="H232" t="s">
         <v>25</v>
       </c>
-      <c r="I232">
+      <c r="I232" s="2">
         <v>44226</v>
       </c>
       <c r="J232" t="s">
@@ -25244,7 +25244,7 @@
       <c r="H233" t="s">
         <v>25</v>
       </c>
-      <c r="I233">
+      <c r="I233" s="2">
         <v>42786</v>
       </c>
       <c r="J233" t="s">
@@ -25306,7 +25306,7 @@
       <c r="H234" t="s">
         <v>25</v>
       </c>
-      <c r="I234">
+      <c r="I234" s="2">
         <v>44494</v>
       </c>
       <c r="J234" t="s">
@@ -25368,7 +25368,7 @@
       <c r="H235" t="s">
         <v>25</v>
       </c>
-      <c r="I235">
+      <c r="I235" s="2">
         <v>43297</v>
       </c>
       <c r="J235" t="s">
@@ -25430,7 +25430,7 @@
       <c r="H236" t="s">
         <v>25</v>
       </c>
-      <c r="I236">
+      <c r="I236" s="2">
         <v>44375</v>
       </c>
       <c r="J236" t="s">
@@ -25492,7 +25492,7 @@
       <c r="H237" t="s">
         <v>25</v>
       </c>
-      <c r="I237">
+      <c r="I237" s="2">
         <v>40224</v>
       </c>
       <c r="J237" t="s">
@@ -25554,7 +25554,7 @@
       <c r="H238" t="s">
         <v>25</v>
       </c>
-      <c r="I238">
+      <c r="I238" s="2">
         <v>44494</v>
       </c>
       <c r="J238" t="s">
@@ -25610,7 +25610,7 @@
       <c r="H239" t="s">
         <v>25</v>
       </c>
-      <c r="I239">
+      <c r="I239" s="2">
         <v>44375</v>
       </c>
       <c r="J239" t="s">
@@ -25672,7 +25672,7 @@
       <c r="H240" t="s">
         <v>25</v>
       </c>
-      <c r="I240">
+      <c r="I240" s="2">
         <v>44494</v>
       </c>
       <c r="J240" t="s">
@@ -25728,7 +25728,7 @@
       <c r="H241" t="s">
         <v>25</v>
       </c>
-      <c r="I241">
+      <c r="I241" s="2">
         <v>44226</v>
       </c>
       <c r="J241" t="s">
@@ -25787,7 +25787,7 @@
       <c r="H242" t="s">
         <v>25</v>
       </c>
-      <c r="I242">
+      <c r="I242" s="2">
         <v>44226</v>
       </c>
       <c r="J242" t="s">
@@ -25846,7 +25846,7 @@
       <c r="H243" t="s">
         <v>25</v>
       </c>
-      <c r="I243">
+      <c r="I243" s="2">
         <v>44229</v>
       </c>
       <c r="J243" t="s">
@@ -25905,7 +25905,7 @@
       <c r="H244" t="s">
         <v>25</v>
       </c>
-      <c r="I244">
+      <c r="I244" s="2">
         <v>44226</v>
       </c>
       <c r="J244" t="s">
@@ -25958,7 +25958,7 @@
       <c r="H245" t="s">
         <v>25</v>
       </c>
-      <c r="I245">
+      <c r="I245" s="2">
         <v>44375</v>
       </c>
       <c r="J245" t="s">
@@ -26014,7 +26014,7 @@
       <c r="H246" t="s">
         <v>25</v>
       </c>
-      <c r="I246">
+      <c r="I246" s="2">
         <v>44494</v>
       </c>
       <c r="J246" t="s">
@@ -26070,7 +26070,7 @@
       <c r="H247" t="s">
         <v>25</v>
       </c>
-      <c r="I247">
+      <c r="I247" s="2">
         <v>44229</v>
       </c>
       <c r="J247" t="s">
@@ -26129,7 +26129,7 @@
       <c r="H248" t="s">
         <v>25</v>
       </c>
-      <c r="I248">
+      <c r="I248" s="2">
         <v>44226</v>
       </c>
       <c r="J248" t="s">
@@ -26191,7 +26191,7 @@
       <c r="H249" t="s">
         <v>25</v>
       </c>
-      <c r="I249">
+      <c r="I249" s="2">
         <v>44375</v>
       </c>
       <c r="J249" t="s">
@@ -26250,7 +26250,7 @@
       <c r="H250" t="s">
         <v>25</v>
       </c>
-      <c r="I250">
+      <c r="I250" s="2">
         <v>44494</v>
       </c>
       <c r="J250" t="s">
@@ -26312,7 +26312,7 @@
       <c r="H251" t="s">
         <v>25</v>
       </c>
-      <c r="I251">
+      <c r="I251" s="2">
         <v>44375</v>
       </c>
       <c r="J251" t="s">
@@ -26371,7 +26371,7 @@
       <c r="H252" t="s">
         <v>25</v>
       </c>
-      <c r="I252">
+      <c r="I252" s="2">
         <v>44226</v>
       </c>
       <c r="J252" t="s">
@@ -26430,7 +26430,7 @@
       <c r="H253" t="s">
         <v>25</v>
       </c>
-      <c r="I253">
+      <c r="I253" s="2">
         <v>44494</v>
       </c>
       <c r="J253" t="s">
@@ -26489,7 +26489,7 @@
       <c r="H254" t="s">
         <v>25</v>
       </c>
-      <c r="I254">
+      <c r="I254" s="2">
         <v>42786</v>
       </c>
       <c r="J254" t="s">
@@ -26548,7 +26548,7 @@
       <c r="H255" t="s">
         <v>25</v>
       </c>
-      <c r="I255">
+      <c r="I255" s="2">
         <v>44494</v>
       </c>
       <c r="J255" t="s">
@@ -26607,7 +26607,7 @@
       <c r="H256" t="s">
         <v>25</v>
       </c>
-      <c r="I256">
+      <c r="I256" s="2">
         <v>44375</v>
       </c>
       <c r="J256" t="s">
@@ -26669,7 +26669,7 @@
       <c r="H257" t="s">
         <v>25</v>
       </c>
-      <c r="I257">
+      <c r="I257" s="2">
         <v>44494</v>
       </c>
       <c r="J257" t="s">
@@ -26731,7 +26731,7 @@
       <c r="H258" t="s">
         <v>25</v>
       </c>
-      <c r="I258">
+      <c r="I258" s="2">
         <v>44076</v>
       </c>
       <c r="J258" t="s">
@@ -26793,7 +26793,7 @@
       <c r="H259" t="s">
         <v>25</v>
       </c>
-      <c r="I259">
+      <c r="I259" s="2">
         <v>44375</v>
       </c>
       <c r="J259" t="s">
@@ -26855,7 +26855,7 @@
       <c r="H260" t="s">
         <v>25</v>
       </c>
-      <c r="I260">
+      <c r="I260" s="2">
         <v>44494</v>
       </c>
       <c r="J260" t="s">
@@ -26914,7 +26914,7 @@
       <c r="H261" t="s">
         <v>25</v>
       </c>
-      <c r="I261">
+      <c r="I261" s="2">
         <v>44494</v>
       </c>
       <c r="J261" t="s">
@@ -26973,7 +26973,7 @@
       <c r="H262" t="s">
         <v>25</v>
       </c>
-      <c r="I262">
+      <c r="I262" s="2">
         <v>44250</v>
       </c>
       <c r="J262" t="s">
@@ -27020,8 +27020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4A0923B-694E-42CA-8075-62B529D9ACDE}">
   <dimension ref="A1:U108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -33384,6 +33384,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>